<commit_message>
tried to add widget?
</commit_message>
<xml_diff>
--- a/assets/data/presentation tracking spreadsheet.xlsx
+++ b/assets/data/presentation tracking spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/scott_coffin_waterboards_ca_gov/Documents/Documents/OFFLINE/DATA/R/GitHub/scottcoffin.github.io/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="748" documentId="8_{057E7423-41A9-4B5A-811C-2C5DD2623C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{520C6FBE-4407-404F-97CD-A040FB65C35F}"/>
+  <xr:revisionPtr revIDLastSave="786" documentId="8_{057E7423-41A9-4B5A-811C-2C5DD2623C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB82BA65-E26F-4922-A700-3F497E6177B7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C88E4DA2-9904-46B4-9B52-E62D75E72379}"/>
+    <workbookView xWindow="22932" yWindow="-2928" windowWidth="23256" windowHeight="12576" xr2:uid="{C88E4DA2-9904-46B4-9B52-E62D75E72379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="202">
   <si>
     <t>Month</t>
   </si>
@@ -3329,6 +3329,108 @@
         <family val="2"/>
       </rPr>
       <t>Managing Microplastics Risks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Southern California Academy of Science: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Risk Characterization of Microplastics in San Francisco Bay, California</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U.S. Government Interest Group on Nanoplastics: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>California's Actions on Microplastics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">AARP: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Plastics and Your Health</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">UC Santa Barbara SNARL Spring Seminar Series: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Microplastics - a Macro Problem?</t>
+    </r>
+  </si>
+  <si>
+    <t>UCR ENTX Seminar Series: Assessing and Managing Risks of Microplastics</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MP Workshop for Early Career Researchers (Athens, Greece):</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Assessing and Managing Risks of Microplastics</t>
     </r>
   </si>
 </sst>
@@ -3471,8 +3573,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:F167" totalsRowShown="0">
-  <autoFilter ref="A1:F167" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:F173" totalsRowShown="0">
+  <autoFilter ref="A1:F173" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}">
     <filterColumn colId="5">
       <filters>
         <filter val="outreach"/>
@@ -3788,10 +3890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACB5D2F-F57D-4559-B66A-28FB60FE7C14}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173:F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7137,6 +7239,126 @@
         <v>153</v>
       </c>
     </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>2022</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D168" t="s">
+        <v>7</v>
+      </c>
+      <c r="E168" t="s">
+        <v>12</v>
+      </c>
+      <c r="F168" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>2022</v>
+      </c>
+      <c r="B169" t="s">
+        <v>14</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D169" t="s">
+        <v>7</v>
+      </c>
+      <c r="E169" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>2022</v>
+      </c>
+      <c r="B170" t="s">
+        <v>14</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D170" t="s">
+        <v>26</v>
+      </c>
+      <c r="E170" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>2022</v>
+      </c>
+      <c r="B171" t="s">
+        <v>14</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D171" t="s">
+        <v>7</v>
+      </c>
+      <c r="E171" t="s">
+        <v>13</v>
+      </c>
+      <c r="F171" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>2022</v>
+      </c>
+      <c r="B172" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D172" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" t="s">
+        <v>12</v>
+      </c>
+      <c r="F172" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>2022</v>
+      </c>
+      <c r="B173" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D173" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" t="s">
+        <v>12</v>
+      </c>
+      <c r="F173" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7147,6 +7369,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA071883F2983240B6E491D588366211" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e55131471194fadee75a71cb0a38fca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5204c27f-60f7-49bb-a536-18f8f47f4373" xmlns:ns4="891bdd1d-ba27-403b-a4cc-21ba34b3f493" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cda03f4a482d0c06e65c8d80cb850303" ns3:_="" ns4:_="">
     <xsd:import namespace="5204c27f-60f7-49bb-a536-18f8f47f4373"/>
@@ -7375,15 +7606,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7391,6 +7613,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914D4EDE-B80A-4C8E-BC45-FFED6152D7FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C6FFEA6-6C1E-4CB8-B09E-6C7754EB6174}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7409,14 +7639,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914D4EDE-B80A-4C8E-BC45-FFED6152D7FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E23BEA-1270-4148-AF2F-F846491CBF06}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated data science page
</commit_message>
<xml_diff>
--- a/assets/data/presentation tracking spreadsheet.xlsx
+++ b/assets/data/presentation tracking spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/scott_coffin_waterboards_ca_gov/Documents/Documents/OFFLINE/DATA/R/GitHub/scottcoffin.github.io/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1132" documentId="8_{057E7423-41A9-4B5A-811C-2C5DD2623C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27CD4918-A150-4BAE-A78F-C070682AAB73}"/>
+  <xr:revisionPtr revIDLastSave="1139" documentId="8_{057E7423-41A9-4B5A-811C-2C5DD2623C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA40FE7A-D312-45AF-BBB6-DF2A839B42DD}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="-2928" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C88E4DA2-9904-46B4-9B52-E62D75E72379}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="256">
   <si>
     <t>Month</t>
   </si>
@@ -4173,6 +4173,9 @@
   </si>
   <si>
     <t>Count of Name</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -4259,7 +4262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4282,7 +4285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6336,7 +6338,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD50137F-1F23-4390-AB5B-CC8B1A215C3B}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD50137F-1F23-4390-AB5B-CC8B1A215C3B}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -6648,21 +6650,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:F219" totalsRowShown="0">
-  <autoFilter ref="A1:F219" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:G219" totalsRowShown="0">
+  <autoFilter ref="A1:G219" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}">
     <filterColumn colId="5">
       <filters>
+        <filter val="lecture"/>
+        <filter val="outreach"/>
         <filter val="podcast"/>
+        <filter val="print"/>
+        <filter val="radio"/>
+        <filter val="television"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{63B172DE-2272-468E-8AEC-649EFF92AC52}" name="Year"/>
     <tableColumn id="2" xr3:uid="{E93EE185-F613-4268-92F9-55DBD6183CCB}" name="Month"/>
     <tableColumn id="3" xr3:uid="{B0DEF885-9E73-460F-8DE8-FF1A54ECE175}" name="Name" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{A9C766C7-5C0E-4C6A-8467-FB45E794EA63}" name="Type"/>
     <tableColumn id="5" xr3:uid="{CE33B0DF-D1F9-4137-98AD-51843C9A962D}" name="Face"/>
     <tableColumn id="6" xr3:uid="{E793D25D-A222-4B24-B9A5-A6FF6233FE31}" name="Category"/>
+    <tableColumn id="7" xr3:uid="{DC423EC5-BA9A-4A00-A26F-8C6CB36CAD58}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6989,7 +6997,7 @@
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>80</v>
       </c>
     </row>
@@ -6997,7 +7005,7 @@
       <c r="A5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>10</v>
       </c>
     </row>
@@ -7005,7 +7013,7 @@
       <c r="A6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>6</v>
       </c>
     </row>
@@ -7013,7 +7021,7 @@
       <c r="A7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>20</v>
       </c>
     </row>
@@ -7021,7 +7029,7 @@
       <c r="A8" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>48</v>
       </c>
     </row>
@@ -7029,7 +7037,7 @@
       <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>33</v>
       </c>
     </row>
@@ -7037,7 +7045,7 @@
       <c r="A10" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>5</v>
       </c>
     </row>
@@ -7045,7 +7053,7 @@
       <c r="A11" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -7053,7 +7061,7 @@
       <c r="A12" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12">
         <v>1</v>
       </c>
     </row>
@@ -7061,7 +7069,7 @@
       <c r="A13" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>3</v>
       </c>
     </row>
@@ -7069,7 +7077,7 @@
       <c r="A14" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14">
         <v>11</v>
       </c>
     </row>
@@ -7077,7 +7085,7 @@
       <c r="A15" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>218</v>
       </c>
     </row>
@@ -7088,10 +7096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACB5D2F-F57D-4559-B66A-28FB60FE7C14}">
-  <dimension ref="A1:F219"/>
+  <dimension ref="A1:G222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" topLeftCell="B172" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7100,7 +7108,7 @@
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7119,8 +7127,11 @@
       <c r="F1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -7140,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -7160,7 +7171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -7180,7 +7191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="17.399999999999999" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -7200,7 +7211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -7220,7 +7231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7240,7 +7251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7260,7 +7271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -7280,7 +7291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -7300,7 +7311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -7320,7 +7331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -7340,7 +7351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -7360,7 +7371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -7380,7 +7391,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -7400,7 +7411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -7740,7 +7751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -7760,7 +7771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -7780,7 +7791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -7800,7 +7811,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -7820,7 +7831,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -7840,7 +7851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -7860,7 +7871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -7880,7 +7891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -7900,7 +7911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -7920,7 +7931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -7940,7 +7951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -7960,7 +7971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2014</v>
       </c>
@@ -7979,8 +7990,11 @@
       <c r="F44" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2015</v>
       </c>
@@ -7999,8 +8013,11 @@
       <c r="F45" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2016</v>
       </c>
@@ -8019,8 +8036,11 @@
       <c r="F46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2016</v>
       </c>
@@ -8039,8 +8059,11 @@
       <c r="F47" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -8059,8 +8082,11 @@
       <c r="F48" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2016</v>
       </c>
@@ -8076,8 +8102,11 @@
       <c r="F49" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2016</v>
       </c>
@@ -8096,8 +8125,11 @@
       <c r="F50" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -8116,8 +8148,11 @@
       <c r="F51" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2018</v>
       </c>
@@ -8136,8 +8171,11 @@
       <c r="F52" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2018</v>
       </c>
@@ -8156,8 +8194,11 @@
       <c r="F53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2018</v>
       </c>
@@ -8176,8 +8217,11 @@
       <c r="F54" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2019</v>
       </c>
@@ -8196,8 +8240,11 @@
       <c r="F55" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -8216,8 +8263,11 @@
       <c r="F56" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2019</v>
       </c>
@@ -8236,8 +8286,11 @@
       <c r="F57" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2020</v>
       </c>
@@ -8256,8 +8309,11 @@
       <c r="F58" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2020</v>
       </c>
@@ -8277,7 +8333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2020</v>
       </c>
@@ -8297,7 +8353,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2020</v>
       </c>
@@ -8317,7 +8373,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2020</v>
       </c>
@@ -8337,7 +8393,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2020</v>
       </c>
@@ -8356,8 +8412,11 @@
       <c r="F63" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2020</v>
       </c>
@@ -8377,7 +8436,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2020</v>
       </c>
@@ -8396,8 +8455,11 @@
       <c r="F65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2020</v>
       </c>
@@ -8417,7 +8479,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2020</v>
       </c>
@@ -8436,8 +8498,11 @@
       <c r="F67" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2020</v>
       </c>
@@ -8457,7 +8522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2020</v>
       </c>
@@ -8476,8 +8541,11 @@
       <c r="F69" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2020</v>
       </c>
@@ -8496,8 +8564,11 @@
       <c r="F70" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2020</v>
       </c>
@@ -8516,8 +8587,11 @@
       <c r="F71" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -8536,8 +8610,11 @@
       <c r="F72" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2020</v>
       </c>
@@ -8556,8 +8633,11 @@
       <c r="F73" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2020</v>
       </c>
@@ -8577,7 +8657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2020</v>
       </c>
@@ -8596,8 +8676,11 @@
       <c r="F75" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2020</v>
       </c>
@@ -8617,7 +8700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -8637,7 +8720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2020</v>
       </c>
@@ -8657,7 +8740,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2020</v>
       </c>
@@ -8677,7 +8760,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2020</v>
       </c>
@@ -8697,7 +8780,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2020</v>
       </c>
@@ -8717,7 +8800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2021</v>
       </c>
@@ -8736,8 +8819,11 @@
       <c r="F82" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2021</v>
       </c>
@@ -8756,8 +8842,11 @@
       <c r="F83" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2021</v>
       </c>
@@ -8777,7 +8866,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2021</v>
       </c>
@@ -8797,7 +8886,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2021</v>
       </c>
@@ -8817,7 +8906,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2021</v>
       </c>
@@ -8837,7 +8926,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2021</v>
       </c>
@@ -8857,7 +8946,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2021</v>
       </c>
@@ -8877,7 +8966,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2021</v>
       </c>
@@ -8897,7 +8986,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2021</v>
       </c>
@@ -8917,7 +9006,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2021</v>
       </c>
@@ -8937,7 +9026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2021</v>
       </c>
@@ -8957,7 +9046,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2021</v>
       </c>
@@ -8977,7 +9066,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2021</v>
       </c>
@@ -8996,8 +9085,11 @@
       <c r="F95" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2021</v>
       </c>
@@ -9017,7 +9109,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2021</v>
       </c>
@@ -9037,7 +9129,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2021</v>
       </c>
@@ -9057,7 +9149,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2021</v>
       </c>
@@ -9077,7 +9169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2021</v>
       </c>
@@ -9097,7 +9189,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2021</v>
       </c>
@@ -9116,8 +9208,11 @@
       <c r="F101" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2021</v>
       </c>
@@ -9137,7 +9232,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2021</v>
       </c>
@@ -9157,7 +9252,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2021</v>
       </c>
@@ -9176,8 +9271,11 @@
       <c r="F104" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2021</v>
       </c>
@@ -9197,7 +9295,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2021</v>
       </c>
@@ -9216,8 +9314,11 @@
       <c r="F106" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2021</v>
       </c>
@@ -9237,7 +9338,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2021</v>
       </c>
@@ -9257,7 +9358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2021</v>
       </c>
@@ -9277,7 +9378,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2021</v>
       </c>
@@ -9297,7 +9398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2021</v>
       </c>
@@ -9316,8 +9417,11 @@
       <c r="F111" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2021</v>
       </c>
@@ -9336,8 +9440,11 @@
       <c r="F112" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2021</v>
       </c>
@@ -9356,8 +9463,11 @@
       <c r="F113" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2021</v>
       </c>
@@ -9377,7 +9487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -9397,7 +9507,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2021</v>
       </c>
@@ -9417,7 +9527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2021</v>
       </c>
@@ -9436,8 +9546,11 @@
       <c r="F117" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2021</v>
       </c>
@@ -9457,7 +9570,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2021</v>
       </c>
@@ -9477,7 +9590,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2021</v>
       </c>
@@ -9496,8 +9609,11 @@
       <c r="F120" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2021</v>
       </c>
@@ -9517,7 +9633,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2021</v>
       </c>
@@ -9537,7 +9653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -9557,7 +9673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2021</v>
       </c>
@@ -9577,7 +9693,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2021</v>
       </c>
@@ -9596,8 +9712,11 @@
       <c r="F125" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2021</v>
       </c>
@@ -9617,7 +9736,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2021</v>
       </c>
@@ -9636,8 +9755,11 @@
       <c r="F127" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2021</v>
       </c>
@@ -9656,8 +9778,11 @@
       <c r="F128" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2021</v>
       </c>
@@ -9677,7 +9802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2021</v>
       </c>
@@ -9697,7 +9822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -9717,7 +9842,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2021</v>
       </c>
@@ -9736,8 +9861,11 @@
       <c r="F132" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2021</v>
       </c>
@@ -9756,8 +9884,11 @@
       <c r="F133" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2021</v>
       </c>
@@ -9776,8 +9907,11 @@
       <c r="F134" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2021</v>
       </c>
@@ -9797,7 +9931,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2021</v>
       </c>
@@ -9817,7 +9951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2021</v>
       </c>
@@ -9837,7 +9971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2021</v>
       </c>
@@ -9857,7 +9991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2021</v>
       </c>
@@ -9877,7 +10011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2021</v>
       </c>
@@ -9897,7 +10031,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2021</v>
       </c>
@@ -9917,7 +10051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2021</v>
       </c>
@@ -9937,7 +10071,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2021</v>
       </c>
@@ -9957,7 +10091,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2022</v>
       </c>
@@ -9977,7 +10111,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2022</v>
       </c>
@@ -9996,8 +10130,11 @@
       <c r="F145" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2022</v>
       </c>
@@ -10017,7 +10154,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2022</v>
       </c>
@@ -10037,7 +10174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2022</v>
       </c>
@@ -10057,7 +10194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2022</v>
       </c>
@@ -10077,7 +10214,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2022</v>
       </c>
@@ -10097,7 +10234,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2022</v>
       </c>
@@ -10117,7 +10254,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2022</v>
       </c>
@@ -10137,7 +10274,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2022</v>
       </c>
@@ -10157,7 +10294,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2022</v>
       </c>
@@ -10177,7 +10314,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2022</v>
       </c>
@@ -10197,7 +10334,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2022</v>
       </c>
@@ -10217,7 +10354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2022</v>
       </c>
@@ -10237,7 +10374,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2022</v>
       </c>
@@ -10257,7 +10394,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2022</v>
       </c>
@@ -10276,8 +10413,11 @@
       <c r="F159" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2022</v>
       </c>
@@ -10296,8 +10436,11 @@
       <c r="F160" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2022</v>
       </c>
@@ -10317,7 +10460,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2022</v>
       </c>
@@ -10337,7 +10480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2022</v>
       </c>
@@ -10357,7 +10500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2022</v>
       </c>
@@ -10377,7 +10520,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2022</v>
       </c>
@@ -10397,7 +10540,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2022</v>
       </c>
@@ -10417,7 +10560,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2022</v>
       </c>
@@ -10436,8 +10579,11 @@
       <c r="F167" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2022</v>
       </c>
@@ -10457,7 +10603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2022</v>
       </c>
@@ -10477,7 +10623,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2022</v>
       </c>
@@ -10497,7 +10643,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2022</v>
       </c>
@@ -10516,8 +10662,11 @@
       <c r="F171" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2022</v>
       </c>
@@ -10536,8 +10685,11 @@
       <c r="F172" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2022</v>
       </c>
@@ -10557,7 +10709,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2022</v>
       </c>
@@ -10576,8 +10728,11 @@
       <c r="F174" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2022</v>
       </c>
@@ -10596,8 +10751,11 @@
       <c r="F175" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2022</v>
       </c>
@@ -10617,7 +10775,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2022</v>
       </c>
@@ -10636,8 +10794,11 @@
       <c r="F177" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2022</v>
       </c>
@@ -10657,7 +10818,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2022</v>
       </c>
@@ -10677,7 +10838,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2022</v>
       </c>
@@ -10697,7 +10858,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2022</v>
       </c>
@@ -10717,7 +10878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2022</v>
       </c>
@@ -10737,7 +10898,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2022</v>
       </c>
@@ -10757,7 +10918,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2022</v>
       </c>
@@ -10777,7 +10938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2022</v>
       </c>
@@ -10796,8 +10957,11 @@
       <c r="F185" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2022</v>
       </c>
@@ -10816,8 +10980,11 @@
       <c r="F186" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2022</v>
       </c>
@@ -10837,7 +11004,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2022</v>
       </c>
@@ -10857,7 +11024,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2022</v>
       </c>
@@ -10877,7 +11044,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2022</v>
       </c>
@@ -10897,7 +11064,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2022</v>
       </c>
@@ -10917,7 +11084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2022</v>
       </c>
@@ -10936,8 +11103,11 @@
       <c r="F192" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2022</v>
       </c>
@@ -10957,7 +11127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2022</v>
       </c>
@@ -10976,8 +11146,11 @@
       <c r="F194" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2022</v>
       </c>
@@ -10997,7 +11170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2022</v>
       </c>
@@ -11017,7 +11190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2022</v>
       </c>
@@ -11037,7 +11210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2022</v>
       </c>
@@ -11057,7 +11230,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2022</v>
       </c>
@@ -11076,8 +11249,11 @@
       <c r="F199" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2022</v>
       </c>
@@ -11096,8 +11272,11 @@
       <c r="F200" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>2022</v>
       </c>
@@ -11117,7 +11296,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>2022</v>
       </c>
@@ -11137,7 +11316,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>2022</v>
       </c>
@@ -11157,7 +11336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2023</v>
       </c>
@@ -11177,7 +11356,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>2023</v>
       </c>
@@ -11197,7 +11376,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>2023</v>
       </c>
@@ -11216,8 +11395,11 @@
       <c r="F206" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>2023</v>
       </c>
@@ -11236,8 +11418,11 @@
       <c r="F207" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>2023</v>
       </c>
@@ -11257,7 +11442,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>2023</v>
       </c>
@@ -11277,7 +11462,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>2023</v>
       </c>
@@ -11297,7 +11482,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>2023</v>
       </c>
@@ -11317,7 +11502,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>2023</v>
       </c>
@@ -11337,7 +11522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>2023</v>
       </c>
@@ -11357,7 +11542,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>2023</v>
       </c>
@@ -11376,8 +11561,11 @@
       <c r="F214" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>2023</v>
       </c>
@@ -11397,7 +11585,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>2023</v>
       </c>
@@ -11416,8 +11604,11 @@
       <c r="F216" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>2023</v>
       </c>
@@ -11436,8 +11627,11 @@
       <c r="F217" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>2023</v>
       </c>
@@ -11456,8 +11650,11 @@
       <c r="F218" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>2023</v>
       </c>
@@ -11475,6 +11672,15 @@
       </c>
       <c r="F219" t="s">
         <v>152</v>
+      </c>
+      <c r="G219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G222">
+        <f>COUNT(G44:G219)</f>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -11487,9 +11693,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11722,19 +11931,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E23BEA-1270-4148-AF2F-F846491CBF06}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914D4EDE-B80A-4C8E-BC45-FFED6152D7FD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11759,9 +11964,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914D4EDE-B80A-4C8E-BC45-FFED6152D7FD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E23BEA-1270-4148-AF2F-F846491CBF06}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated talks spreadsheet and plotly
</commit_message>
<xml_diff>
--- a/assets/data/presentation tracking spreadsheet.xlsx
+++ b/assets/data/presentation tracking spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/scott_coffin_waterboards_ca_gov/Documents/Documents/OFFLINE/DATA/R/GitHub/scottcoffin.github.io/assets/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott.Coffin\OneDrive - California OEHHA\R_new\scottcoffin.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1258" documentId="8_{057E7423-41A9-4B5A-811C-2C5DD2623C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4D2CA4A-E0E2-4FA0-8FFB-F533D76719A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C07F78A-4C65-41FD-ADC4-273382F629EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C88E4DA2-9904-46B4-9B52-E62D75E72379}"/>
+    <workbookView xWindow="57480" yWindow="630" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{C88E4DA2-9904-46B4-9B52-E62D75E72379}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="306">
   <si>
     <t>Month</t>
   </si>
@@ -4243,6 +4243,102 @@
   </si>
   <si>
     <t>USEPA Trash Free Waters: Nano- and Microplastics Webinar</t>
+  </si>
+  <si>
+    <t>DSU Roundtable: State Water Board Actions on Microplastics</t>
+  </si>
+  <si>
+    <t>Water Quality Monitoring Council: The State Water Board's Microplastics in Drinking Water Monitoring Plan</t>
+  </si>
+  <si>
+    <t>Water Quality Monitoring Council: Microplastics Monitoring: The Big Picture (a.k.a. where do we go from here?)</t>
+  </si>
+  <si>
+    <t>WRF 5185 - Unit Process Targeting Workshop: The State Water Board's Microplastics in Drinking Water Monitoring Plan</t>
+  </si>
+  <si>
+    <t>Advancing Understanding: Exploring Current Research and Bridging Knowledge Gaps in Microplastics Science: California's Microplastics Drinking Water Monitoring Program</t>
+  </si>
+  <si>
+    <t>IJC Workshop on Ecological Risk Assessment for Microplastics: Re-scaling and Aligning Exposure and Hazard Data to enable Reliable Comparisons</t>
+  </si>
+  <si>
+    <t>California Water Quality Monitoring Council: Microplastics Monitoring Subcommittee Meeting</t>
+  </si>
+  <si>
+    <t>American Clean Water Association Groundwater Quality Subcommittee: Monitoring and Managing Risks of Microplastics in California's Drinking Wate: Knowns and Unkowns of Groundwater</t>
+  </si>
+  <si>
+    <t>Digital Art Workshop Retreat: Think like a scientist communicate like an artist: the art of storytelling in science communication</t>
+  </si>
+  <si>
+    <t>Tahoe Council Science Advisory Council: California Environmental Protection Agency's Research and Actions on Microplastics</t>
+  </si>
+  <si>
+    <t>Digital Art Workshop Retreat: Generative AI Image Production</t>
+  </si>
+  <si>
+    <t>American Geosciences Institute Earth Day Webinar: California's Adaptive Risk Management of Microplastics in Aquatic Ecosystems and Drinking Water</t>
+  </si>
+  <si>
+    <t>FoolsFest 2024: Some Bits I've Learned about Science Communication</t>
+  </si>
+  <si>
+    <t>California Lake Management Society: Risk Management Strategies for Microplastics in Aquatic Environments</t>
+  </si>
+  <si>
+    <t>OEHHA Journal Club: Test Methods to Evaluate Ecological Safety of 6-PPQ-Quinone and its Alternatives</t>
+  </si>
+  <si>
+    <t>American Chemical Society San Diego Chapter: The Science of Microplastics: Impacts on Health and Ecosystems</t>
+  </si>
+  <si>
+    <t>Los Angeles County Bar Association: Microplastics webinar</t>
+  </si>
+  <si>
+    <t>Cheyenne Rotary Club: Understanding and Addressing Environmental Impacts of Microplastics</t>
+  </si>
+  <si>
+    <t>Central Coast Regional Water Quality Control Board: Addressing Impacts of Microplastics on Aquatic Ecosystems</t>
+  </si>
+  <si>
+    <t>NAMs Discussion Club: New approach methods to evaluate safer alternatives to a lethal tire additive</t>
+  </si>
+  <si>
+    <t>Honor Society of Food Science &amp; Technology Webinar: Microplastics and Nanoplastics in Water and the Environment</t>
+  </si>
+  <si>
+    <t>UC Riverside Graduate Professional Development Course: A Day in the Life of a CalEPA Research Scientist</t>
+  </si>
+  <si>
+    <t>Workshop on Drinking Water Sample Collection Methods for Micorplastics - Health Effects</t>
+  </si>
+  <si>
+    <t>Health Officers Association of California: Findings from the State Water Board's Health Effects Working Group on Microplastics</t>
+  </si>
+  <si>
+    <t>American Water Works Association Webinar: Findings from the State Water Board's Health Effects Working Group on Microplastics</t>
+  </si>
+  <si>
+    <t>Microfibre Textile Sail: Impacts of Microfiber &amp; Chemical Pollution</t>
+  </si>
+  <si>
+    <t>Associated of Public Health Laboratories 2025 Annual Conference: Monitoringh and Assessing Risks of Microplastics - Insights from California</t>
+  </si>
+  <si>
+    <t>PWRPNT Party: Microplastics: the Misunderstood Macronutrient</t>
+  </si>
+  <si>
+    <t>Microplastic Pollution: Impacts on the SF Bay Delta and Remediation Strategies (UC Davis): A Comprehensive Probabilistic Framework for Deriving Microplastic Hazard Thresholds: Development and Application to Marine and Freshwater Ecosystems with ToMEx 2.0 Data</t>
+  </si>
+  <si>
+    <t>GitHub 101</t>
+  </si>
+  <si>
+    <t>Gordon Research Conference - Environmental Nanotechnology. Challenges and Advances in Assessing Ecological Risks of Microplastics: Findings from a Large International Working Group's Meta-Analysis</t>
+  </si>
+  <si>
+    <t>Internal Microplastics Briefing (OEHHA)</t>
   </si>
 </sst>
 </file>
@@ -4317,7 +4413,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4325,11 +4421,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4352,6 +4472,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4389,18 +4516,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Coffin, Scott@Waterboards" refreshedDate="45257.63728599537" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="235" xr:uid="{4E2DABD9-38D0-4889-96F6-B3F28CD0EC34}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Coffin, Scott@OEHHA" refreshedDate="45912.716353587966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="269" xr:uid="{4E2DABD9-38D0-4889-96F6-B3F28CD0EC34}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2023"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2025"/>
     </cacheField>
     <cacheField name="Month" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -4430,7 +4553,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Column1" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="79"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -4442,7 +4565,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="235">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="269">
   <r>
     <n v="2015"/>
     <s v="November"/>
@@ -6558,11 +6681,317 @@
     <x v="7"/>
     <m/>
   </r>
+  <r>
+    <n v="2023"/>
+    <s v="November"/>
+    <s v="USEPA Trash Free Waters: Nano- and Microplastics Webinar"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2023"/>
+    <s v="December"/>
+    <s v="DSU Roundtable: State Water Board Actions on Microplastics"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2023"/>
+    <s v="December"/>
+    <s v="Water Quality Monitoring Council: The State Water Board's Microplastics in Drinking Water Monitoring Plan"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2023"/>
+    <s v="December"/>
+    <s v="Water Quality Monitoring Council: Microplastics Monitoring: The Big Picture (a.k.a. where do we go from here?)"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="5"/>
+    <n v="79"/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="January"/>
+    <s v="WRF 5185 - Unit Process Targeting Workshop: The State Water Board's Microplastics in Drinking Water Monitoring Plan"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="January"/>
+    <s v="Advancing Understanding: Exploring Current Research and Bridging Knowledge Gaps in Microplastics Science: California's Microplastics Drinking Water Monitoring Program"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="January"/>
+    <s v="IJC Workshop on Ecological Risk Assessment for Microplastics: Re-scaling and Aligning Exposure and Hazard Data to enable Reliable Comparisons"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="January"/>
+    <s v="California Water Quality Monitoring Council: Microplastics Monitoring Subcommittee Meeting"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="February"/>
+    <s v="American Clean Water Association Groundwater Quality Subcommittee: Monitoring and Managing Risks of Microplastics in California's Drinking Wate: Knowns and Unkowns of Groundwater"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="February"/>
+    <s v="Digital Art Workshop Retreat: Think like a scientist communicate like an artist: the art of storytelling in science communication"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="February"/>
+    <s v="Tahoe Council Science Advisory Council: California Environmental Protection Agency's Research and Actions on Microplastics"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="February"/>
+    <s v="Digital Art Workshop Retreat: Generative AI Image Production"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="April"/>
+    <s v="American Geosciences Institute Earth Day Webinar: California's Adaptive Risk Management of Microplastics in Aquatic Ecosystems and Drinking Water"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="March"/>
+    <s v="FoolsFest 2024: Some Bits I've Learned about Science Communication"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="April"/>
+    <s v="California Lake Management Society: Risk Management Strategies for Microplastics in Aquatic Environments"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="May"/>
+    <s v="OEHHA Journal Club: Test Methods to Evaluate Ecological Safety of 6-PPQ-Quinone and its Alternatives"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="May"/>
+    <s v="American Chemical Society San Diego Chapter: The Science of Microplastics: Impacts on Health and Ecosystems"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="June"/>
+    <s v="Los Angeles County Bar Association: Microplastics webinar"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="July"/>
+    <s v="Cheyenne Rotary Club: Understanding and Addressing Environmental Impacts of Microplastics"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="August"/>
+    <s v="Central Coast Regional Water Quality Control Board: Addressing Impacts of Microplastics on Aquatic Ecosystems"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="August"/>
+    <s v="NAMs Discussion Club: New approach methods to evaluate safer alternatives to a lethal tire additive"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="October"/>
+    <s v="Honor Society of Food Science &amp; Technology Webinar: Microplastics and Nanoplastics in Water and the Environment"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="November"/>
+    <s v="California Water Quality Monitoring Council: Microplastics Monitoring Subcommittee Meeting"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2024"/>
+    <s v="December"/>
+    <s v="UC Riverside Graduate Professional Development Course: A Day in the Life of a CalEPA Research Scientist"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="4"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="February"/>
+    <s v="Workshop on Drinking Water Sample Collection Methods for Micorplastics - Health Effects"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="5"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="March"/>
+    <s v="Health Officers Association of California: Findings from the State Water Board's Health Effects Working Group on Microplastics"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="April"/>
+    <s v="American Water Works Association Webinar: Findings from the State Water Board's Health Effects Working Group on Microplastics"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="7"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="April"/>
+    <s v="Microfibre Textile Sail: Impacts of Microfiber &amp; Chemical Pollution"/>
+    <s v="other"/>
+    <s v="in person"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="May"/>
+    <s v="Associated of Public Health Laboratories 2025 Annual Conference: Monitoringh and Assessing Risks of Microplastics - Insights from California"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="April"/>
+    <s v="PWRPNT Party: Microplastics: the Misunderstood Macronutrient"/>
+    <s v="other"/>
+    <s v="in person"/>
+    <x v="3"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="May"/>
+    <s v="Microplastic Pollution: Impacts on the SF Bay Delta and Remediation Strategies (UC Davis): A Comprehensive Probabilistic Framework for Deriving Microplastic Hazard Thresholds: Development and Application to Marine and Freshwater Ecosystems with ToMEx 2.0 Data"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="March"/>
+    <s v="GitHub 101"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="4"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="June"/>
+    <s v="Gordon Research Conference - Environmental Nanotechnology. Challenges and Advances in Assessing Ecological Risks of Microplastics: Findings from a Large International Working Group's Meta-Analysis"/>
+    <s v="Platform"/>
+    <s v="in person"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="2025"/>
+    <s v="August"/>
+    <s v="Internal Microplastics Briefing (OEHHA)"/>
+    <s v="Platform"/>
+    <s v="virtual"/>
+    <x v="5"/>
+    <m/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD50137F-1F23-4390-AB5B-CC8B1A215C3B}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD50137F-1F23-4390-AB5B-CC8B1A215C3B}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6648,8 +7077,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:G237" totalsRowShown="0">
-  <autoFilter ref="A1:G237" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{431CEEEE-931D-484C-8E07-C5C4C4AF21DA}" name="Table1" displayName="Table1" ref="A1:G270" totalsRowShown="0">
+  <autoFilter ref="A1:G270" xr:uid="{C328BEFC-0659-480C-8EB4-C9284396A2D2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{63B172DE-2272-468E-8AEC-649EFF92AC52}" name="Year"/>
     <tableColumn id="2" xr3:uid="{E93EE185-F613-4268-92F9-55DBD6183CCB}" name="Month"/>
@@ -6664,9 +7093,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6704,7 +7133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6810,7 +7239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6952,7 +7381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6960,20 +7389,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACB5D2F-F57D-4559-B66A-28FB60FE7C14}">
-  <dimension ref="A1:G240"/>
+  <dimension ref="A1:G270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G237" sqref="G237"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B271" sqref="B271"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="147.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="147.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6996,7 +7428,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -7016,7 +7448,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -7036,7 +7468,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -7056,7 +7488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -7076,7 +7508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -7096,7 +7528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -7116,7 +7548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -7136,7 +7568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -7156,7 +7588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -7176,7 +7608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -7196,7 +7628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -7216,7 +7648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -7236,7 +7668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -7259,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -7279,7 +7711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -7299,7 +7731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -7319,7 +7751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -7339,7 +7771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -7359,7 +7791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -7379,7 +7811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2021</v>
       </c>
@@ -7399,7 +7831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -7419,7 +7851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -7439,7 +7871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -7459,7 +7891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -7479,7 +7911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -7499,7 +7931,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -7519,7 +7951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -7539,7 +7971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -7559,7 +7991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -7579,7 +8011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2021</v>
       </c>
@@ -7599,7 +8031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2021</v>
       </c>
@@ -7619,7 +8051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -7639,7 +8071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -7659,7 +8091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -7682,7 +8114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -7702,7 +8134,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -7722,7 +8154,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -7742,7 +8174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -7762,7 +8194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -7782,7 +8214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -7802,7 +8234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -7822,7 +8254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -7842,7 +8274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2014</v>
       </c>
@@ -7865,7 +8297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2015</v>
       </c>
@@ -7888,7 +8320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2016</v>
       </c>
@@ -7911,7 +8343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2016</v>
       </c>
@@ -7934,7 +8366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2016</v>
       </c>
@@ -7957,7 +8389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2016</v>
       </c>
@@ -7977,7 +8409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2016</v>
       </c>
@@ -8000,7 +8432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -8023,7 +8455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2018</v>
       </c>
@@ -8046,7 +8478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2018</v>
       </c>
@@ -8069,7 +8501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2018</v>
       </c>
@@ -8092,7 +8524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2019</v>
       </c>
@@ -8115,7 +8547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -8138,7 +8570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2019</v>
       </c>
@@ -8161,7 +8593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2020</v>
       </c>
@@ -8184,7 +8616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2020</v>
       </c>
@@ -8204,7 +8636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2020</v>
       </c>
@@ -8224,7 +8656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2020</v>
       </c>
@@ -8244,7 +8676,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2020</v>
       </c>
@@ -8264,7 +8696,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2020</v>
       </c>
@@ -8287,7 +8719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2020</v>
       </c>
@@ -8307,7 +8739,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2020</v>
       </c>
@@ -8330,7 +8762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2020</v>
       </c>
@@ -8350,7 +8782,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2020</v>
       </c>
@@ -8373,7 +8805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2020</v>
       </c>
@@ -8393,7 +8825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2020</v>
       </c>
@@ -8416,7 +8848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2020</v>
       </c>
@@ -8439,7 +8871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2020</v>
       </c>
@@ -8462,7 +8894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -8485,7 +8917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2020</v>
       </c>
@@ -8508,7 +8940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2020</v>
       </c>
@@ -8528,7 +8960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2020</v>
       </c>
@@ -8551,7 +8983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2020</v>
       </c>
@@ -8571,7 +9003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -8591,7 +9023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2020</v>
       </c>
@@ -8611,7 +9043,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2020</v>
       </c>
@@ -8631,7 +9063,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2020</v>
       </c>
@@ -8651,7 +9083,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2020</v>
       </c>
@@ -8671,7 +9103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2021</v>
       </c>
@@ -8694,7 +9126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2021</v>
       </c>
@@ -8717,7 +9149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2021</v>
       </c>
@@ -8737,7 +9169,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2021</v>
       </c>
@@ -8757,7 +9189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2021</v>
       </c>
@@ -8777,7 +9209,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2021</v>
       </c>
@@ -8797,7 +9229,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2021</v>
       </c>
@@ -8817,7 +9249,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2021</v>
       </c>
@@ -8837,7 +9269,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2021</v>
       </c>
@@ -8857,7 +9289,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2021</v>
       </c>
@@ -8877,7 +9309,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2021</v>
       </c>
@@ -8897,7 +9329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2021</v>
       </c>
@@ -8917,7 +9349,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2021</v>
       </c>
@@ -8937,7 +9369,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2021</v>
       </c>
@@ -8960,7 +9392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2021</v>
       </c>
@@ -8980,7 +9412,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2021</v>
       </c>
@@ -9000,7 +9432,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2021</v>
       </c>
@@ -9020,7 +9452,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2021</v>
       </c>
@@ -9040,7 +9472,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2021</v>
       </c>
@@ -9060,7 +9492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2021</v>
       </c>
@@ -9083,7 +9515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2021</v>
       </c>
@@ -9103,7 +9535,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2021</v>
       </c>
@@ -9123,7 +9555,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2021</v>
       </c>
@@ -9146,7 +9578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2021</v>
       </c>
@@ -9166,7 +9598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2021</v>
       </c>
@@ -9189,7 +9621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2021</v>
       </c>
@@ -9209,7 +9641,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2021</v>
       </c>
@@ -9229,7 +9661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2021</v>
       </c>
@@ -9249,7 +9681,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2021</v>
       </c>
@@ -9269,7 +9701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2021</v>
       </c>
@@ -9292,7 +9724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2021</v>
       </c>
@@ -9315,7 +9747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2021</v>
       </c>
@@ -9338,7 +9770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2021</v>
       </c>
@@ -9358,7 +9790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -9378,7 +9810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2021</v>
       </c>
@@ -9398,7 +9830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2021</v>
       </c>
@@ -9421,7 +9853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2021</v>
       </c>
@@ -9441,7 +9873,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2021</v>
       </c>
@@ -9461,7 +9893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2021</v>
       </c>
@@ -9484,7 +9916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2021</v>
       </c>
@@ -9504,7 +9936,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2021</v>
       </c>
@@ -9524,7 +9956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -9544,7 +9976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2021</v>
       </c>
@@ -9564,7 +9996,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2021</v>
       </c>
@@ -9587,7 +10019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2021</v>
       </c>
@@ -9607,7 +10039,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2021</v>
       </c>
@@ -9630,7 +10062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2021</v>
       </c>
@@ -9653,7 +10085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2021</v>
       </c>
@@ -9673,7 +10105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2021</v>
       </c>
@@ -9693,7 +10125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -9713,7 +10145,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2021</v>
       </c>
@@ -9736,7 +10168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2021</v>
       </c>
@@ -9759,7 +10191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2021</v>
       </c>
@@ -9782,7 +10214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2021</v>
       </c>
@@ -9802,7 +10234,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2021</v>
       </c>
@@ -9822,7 +10254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2021</v>
       </c>
@@ -9842,7 +10274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2021</v>
       </c>
@@ -9862,7 +10294,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2021</v>
       </c>
@@ -9882,7 +10314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2021</v>
       </c>
@@ -9902,7 +10334,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2021</v>
       </c>
@@ -9922,7 +10354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2021</v>
       </c>
@@ -9942,7 +10374,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2021</v>
       </c>
@@ -9962,7 +10394,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2022</v>
       </c>
@@ -9982,7 +10414,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2022</v>
       </c>
@@ -10005,7 +10437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2022</v>
       </c>
@@ -10025,7 +10457,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2022</v>
       </c>
@@ -10045,7 +10477,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2022</v>
       </c>
@@ -10065,7 +10497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2022</v>
       </c>
@@ -10085,7 +10517,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2022</v>
       </c>
@@ -10105,7 +10537,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2022</v>
       </c>
@@ -10125,7 +10557,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2022</v>
       </c>
@@ -10145,7 +10577,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2022</v>
       </c>
@@ -10165,7 +10597,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2022</v>
       </c>
@@ -10185,7 +10617,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2022</v>
       </c>
@@ -10205,7 +10637,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2022</v>
       </c>
@@ -10225,7 +10657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2022</v>
       </c>
@@ -10245,7 +10677,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2022</v>
       </c>
@@ -10265,7 +10697,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2022</v>
       </c>
@@ -10288,7 +10720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2022</v>
       </c>
@@ -10311,7 +10743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2022</v>
       </c>
@@ -10331,7 +10763,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2022</v>
       </c>
@@ -10351,7 +10783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2022</v>
       </c>
@@ -10371,7 +10803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2022</v>
       </c>
@@ -10391,7 +10823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2022</v>
       </c>
@@ -10414,7 +10846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2022</v>
       </c>
@@ -10434,7 +10866,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2022</v>
       </c>
@@ -10457,7 +10889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2022</v>
       </c>
@@ -10477,7 +10909,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2022</v>
       </c>
@@ -10497,7 +10929,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2022</v>
       </c>
@@ -10517,7 +10949,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2022</v>
       </c>
@@ -10540,7 +10972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2022</v>
       </c>
@@ -10563,7 +10995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2022</v>
       </c>
@@ -10583,7 +11015,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2022</v>
       </c>
@@ -10606,7 +11038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2022</v>
       </c>
@@ -10629,7 +11061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2022</v>
       </c>
@@ -10649,7 +11081,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2022</v>
       </c>
@@ -10672,7 +11104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2022</v>
       </c>
@@ -10692,7 +11124,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2022</v>
       </c>
@@ -10715,7 +11147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2022</v>
       </c>
@@ -10738,7 +11170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2022</v>
       </c>
@@ -10758,7 +11190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2022</v>
       </c>
@@ -10778,7 +11210,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2022</v>
       </c>
@@ -10798,7 +11230,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2022</v>
       </c>
@@ -10818,7 +11250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2022</v>
       </c>
@@ -10841,7 +11273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2022</v>
       </c>
@@ -10864,7 +11296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2022</v>
       </c>
@@ -10884,7 +11316,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2022</v>
       </c>
@@ -10904,7 +11336,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2022</v>
       </c>
@@ -10927,7 +11359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2022</v>
       </c>
@@ -10947,7 +11379,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2022</v>
       </c>
@@ -10967,7 +11399,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2022</v>
       </c>
@@ -10990,7 +11422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2022</v>
       </c>
@@ -11013,7 +11445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2022</v>
       </c>
@@ -11036,7 +11468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2022</v>
       </c>
@@ -11056,7 +11488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2022</v>
       </c>
@@ -11076,7 +11508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2022</v>
       </c>
@@ -11096,7 +11528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2022</v>
       </c>
@@ -11116,7 +11548,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2022</v>
       </c>
@@ -11139,7 +11571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2022</v>
       </c>
@@ -11162,7 +11594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>2022</v>
       </c>
@@ -11185,7 +11617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>2022</v>
       </c>
@@ -11208,7 +11640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>2022</v>
       </c>
@@ -11228,7 +11660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2023</v>
       </c>
@@ -11248,7 +11680,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>2023</v>
       </c>
@@ -11268,7 +11700,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>2023</v>
       </c>
@@ -11291,7 +11723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>2023</v>
       </c>
@@ -11314,7 +11746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>2023</v>
       </c>
@@ -11334,7 +11766,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>2023</v>
       </c>
@@ -11354,7 +11786,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>2023</v>
       </c>
@@ -11374,7 +11806,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>2023</v>
       </c>
@@ -11397,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>2023</v>
       </c>
@@ -11417,7 +11849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>2023</v>
       </c>
@@ -11437,7 +11869,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>2023</v>
       </c>
@@ -11460,7 +11892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>2023</v>
       </c>
@@ -11480,7 +11912,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>2023</v>
       </c>
@@ -11503,7 +11935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>2023</v>
       </c>
@@ -11526,7 +11958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>2023</v>
       </c>
@@ -11549,7 +11981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>2023</v>
       </c>
@@ -11572,7 +12004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>2023</v>
       </c>
@@ -11595,7 +12027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>2023</v>
       </c>
@@ -11618,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>2023</v>
       </c>
@@ -11641,7 +12073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>2023</v>
       </c>
@@ -11661,7 +12093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>2023</v>
       </c>
@@ -11684,7 +12116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>2023</v>
       </c>
@@ -11704,7 +12136,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>2023</v>
       </c>
@@ -11724,7 +12156,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>2023</v>
       </c>
@@ -11744,7 +12176,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>2023</v>
       </c>
@@ -11764,7 +12196,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>2023</v>
       </c>
@@ -11784,7 +12216,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>2023</v>
       </c>
@@ -11804,7 +12236,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>2023</v>
       </c>
@@ -11824,7 +12256,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>2023</v>
       </c>
@@ -11847,7 +12279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>2023</v>
       </c>
@@ -11870,7 +12302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>2023</v>
       </c>
@@ -11890,7 +12322,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>2023</v>
       </c>
@@ -11910,7 +12342,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>2023</v>
       </c>
@@ -11930,7 +12362,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>2023</v>
       </c>
@@ -11950,10 +12382,668 @@
         <v>203</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>2023</v>
+      </c>
+      <c r="B238" t="s">
+        <v>18</v>
+      </c>
+      <c r="C238" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D238" t="s">
+        <v>7</v>
+      </c>
+      <c r="E238" t="s">
+        <v>13</v>
+      </c>
+      <c r="F238" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>2023</v>
+      </c>
+      <c r="B239" t="s">
+        <v>18</v>
+      </c>
+      <c r="C239" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D239" t="s">
+        <v>7</v>
+      </c>
+      <c r="E239" t="s">
+        <v>12</v>
+      </c>
+      <c r="F239" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A240" s="12">
+        <v>2023</v>
+      </c>
+      <c r="B240" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C240" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D240" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E240" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F240" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="G240">
         <f>SUM(G14:G233)</f>
         <v>79</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>2024</v>
+      </c>
+      <c r="B241" t="s">
+        <v>19</v>
+      </c>
+      <c r="C241" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D241" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E241" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F241" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>2024</v>
+      </c>
+      <c r="B242" t="s">
+        <v>19</v>
+      </c>
+      <c r="C242" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D242" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E242" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F242" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>2024</v>
+      </c>
+      <c r="B243" t="s">
+        <v>19</v>
+      </c>
+      <c r="C243" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D243" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E243" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F243" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>2024</v>
+      </c>
+      <c r="B244" t="s">
+        <v>19</v>
+      </c>
+      <c r="C244" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D244" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E244" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F244" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>2024</v>
+      </c>
+      <c r="B245" t="s">
+        <v>10</v>
+      </c>
+      <c r="C245" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D245" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E245" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F245" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>2024</v>
+      </c>
+      <c r="B246" t="s">
+        <v>10</v>
+      </c>
+      <c r="C246" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D246" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E246" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F246" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>2024</v>
+      </c>
+      <c r="B247" t="s">
+        <v>10</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D247" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E247" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F247" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>2024</v>
+      </c>
+      <c r="B248" t="s">
+        <v>10</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D248" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E248" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F248" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>2024</v>
+      </c>
+      <c r="B249" t="s">
+        <v>6</v>
+      </c>
+      <c r="C249" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D249" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E249" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F249" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>2024</v>
+      </c>
+      <c r="B250" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D250" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E250" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F250" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>2024</v>
+      </c>
+      <c r="B251" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D251" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E251" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F251" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>2024</v>
+      </c>
+      <c r="B252" t="s">
+        <v>14</v>
+      </c>
+      <c r="C252" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D252" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E252" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F252" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>2024</v>
+      </c>
+      <c r="B253" t="s">
+        <v>14</v>
+      </c>
+      <c r="C253" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D253" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E253" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F253" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>2024</v>
+      </c>
+      <c r="B254" t="s">
+        <v>8</v>
+      </c>
+      <c r="C254" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D254" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E254" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F254" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>2024</v>
+      </c>
+      <c r="B255" t="s">
+        <v>20</v>
+      </c>
+      <c r="C255" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D255" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E255" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F255" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>2024</v>
+      </c>
+      <c r="B256" t="s">
+        <v>15</v>
+      </c>
+      <c r="C256" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D256" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E256" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F256" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>2024</v>
+      </c>
+      <c r="B257" t="s">
+        <v>15</v>
+      </c>
+      <c r="C257" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D257" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E257" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F257" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>2024</v>
+      </c>
+      <c r="B258" t="s">
+        <v>17</v>
+      </c>
+      <c r="C258" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D258" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E258" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F258" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>2024</v>
+      </c>
+      <c r="B259" t="s">
+        <v>5</v>
+      </c>
+      <c r="C259" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D259" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E259" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F259" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>2024</v>
+      </c>
+      <c r="B260" t="s">
+        <v>18</v>
+      </c>
+      <c r="C260" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D260" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E260" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F260" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>2025</v>
+      </c>
+      <c r="B261" t="s">
+        <v>10</v>
+      </c>
+      <c r="C261" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D261" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E261" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F261" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>2025</v>
+      </c>
+      <c r="B262" t="s">
+        <v>9</v>
+      </c>
+      <c r="C262" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D262" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E262" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F262" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>2025</v>
+      </c>
+      <c r="B263" t="s">
+        <v>6</v>
+      </c>
+      <c r="C263" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D263" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E263" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F263" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>2025</v>
+      </c>
+      <c r="B264" t="s">
+        <v>6</v>
+      </c>
+      <c r="C264" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D264" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E264" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F264" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>2025</v>
+      </c>
+      <c r="B265" t="s">
+        <v>14</v>
+      </c>
+      <c r="C265" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D265" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E265" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F265" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>2025</v>
+      </c>
+      <c r="B266" t="s">
+        <v>6</v>
+      </c>
+      <c r="C266" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="D266" t="s">
+        <v>25</v>
+      </c>
+      <c r="E266" t="s">
+        <v>12</v>
+      </c>
+      <c r="F266" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>2025</v>
+      </c>
+      <c r="B267" t="s">
+        <v>14</v>
+      </c>
+      <c r="C267" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D267" t="s">
+        <v>7</v>
+      </c>
+      <c r="E267" t="s">
+        <v>12</v>
+      </c>
+      <c r="F267" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>2025</v>
+      </c>
+      <c r="B268" t="s">
+        <v>9</v>
+      </c>
+      <c r="C268" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D268" t="s">
+        <v>7</v>
+      </c>
+      <c r="E268" t="s">
+        <v>13</v>
+      </c>
+      <c r="F268" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>2025</v>
+      </c>
+      <c r="B269" t="s">
+        <v>8</v>
+      </c>
+      <c r="C269" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D269" t="s">
+        <v>7</v>
+      </c>
+      <c r="E269" t="s">
+        <v>12</v>
+      </c>
+      <c r="F269" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>2025</v>
+      </c>
+      <c r="B270" t="s">
+        <v>15</v>
+      </c>
+      <c r="C270" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D270" t="s">
+        <v>7</v>
+      </c>
+      <c r="E270" t="s">
+        <v>13</v>
+      </c>
+      <c r="F270" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -11969,17 +13059,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB154E5-AD5C-4DCF-9875-7F8B258FFC06}">
   <dimension ref="A3:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>252</v>
       </c>
@@ -11987,100 +13077,100 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B8">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B15">
-        <v>235</v>
+      <c r="B15" s="16">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -12098,6 +13188,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA071883F2983240B6E491D588366211" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e55131471194fadee75a71cb0a38fca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5204c27f-60f7-49bb-a536-18f8f47f4373" xmlns:ns4="891bdd1d-ba27-403b-a4cc-21ba34b3f493" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cda03f4a482d0c06e65c8d80cb850303" ns3:_="" ns4:_="">
     <xsd:import namespace="5204c27f-60f7-49bb-a536-18f8f47f4373"/>
@@ -12326,12 +13422,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914D4EDE-B80A-4C8E-BC45-FFED6152D7FD}">
   <ds:schemaRefs>
@@ -12341,6 +13431,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E23BEA-1270-4148-AF2F-F846491CBF06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C6FFEA6-6C1E-4CB8-B09E-6C7754EB6174}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12357,13 +13456,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60E23BEA-1270-4148-AF2F-F846491CBF06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>